<commit_message>
REPORTGEN-700: fix owasp reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/OWASP-2013 Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/OWASP-2013 Full Detailed Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF325AF-8D77-4364-A4AA-23972F5EDBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B19B4B-BB35-4E65-B7A9-BFA3420A34E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=OWASP-2013</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A1-2013</t>
-  </si>
-  <si>
     <t>CAST findings for A1 - Injection</t>
   </si>
   <si>
@@ -128,12 +125,6 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A2-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A2-2013</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A3-2013</t>
-  </si>
-  <si>
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A3-2013,COUNT=-1</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A4-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A4-2013</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAST findings details for A4- Insecure Direct Object References </t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A5-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A5-2013</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAST findings for A5 – Security Misconfiguration </t>
   </si>
   <si>
@@ -170,9 +155,6 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A6-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A6-2013</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAST findings for A6 – Sensitive Data Exposure </t>
   </si>
   <si>
@@ -182,9 +164,6 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A7-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A7-2013</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAST findings for A7 – Missing Function Level Access Control </t>
   </si>
   <si>
@@ -194,18 +173,12 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A8-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A8-2013</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAST findings for A8 – Cross site Request Forgery </t>
   </si>
   <si>
     <t xml:space="preserve">CAST findings details for A8 – Cross site Request Forgery </t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A9-2013</t>
-  </si>
-  <si>
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A9-2013,COUNT=-1</t>
   </si>
   <si>
@@ -218,13 +191,40 @@
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=A10-2013,COUNT=-1</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=A10-2013</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAST findings for A10 – Using Unvalidated Redirects &amp; Forwards </t>
   </si>
   <si>
     <t xml:space="preserve">CAST findings details for A10 – Using Unvalidated Redirects &amp; Forwards </t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A1-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A2-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A3-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A4-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A5-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A6-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A7-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A8-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A9-2013</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=A10-2013</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
   <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,7 +996,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7E084B-1D41-49A1-AAE8-65E5FD99EAE8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1009,12 +1011,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1037,12 +1039,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1055,7 +1057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6184CFD3-505D-44C0-8258-50A02CF4F83B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1068,12 +1072,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1096,12 +1100,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40429C24-E986-40B1-9C54-93D6527149C0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1127,12 +1133,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EB8EA9-CBE4-4B5D-A35C-7E148B322568}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1155,12 +1163,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1174,7 +1182,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,12 +1196,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1218,12 +1226,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1244,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBA7DBA-4263-4117-BE33-EEC6555217AC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1249,12 +1259,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1277,12 +1287,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1310,12 +1320,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1329,7 +1339,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1343,12 +1353,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1373,12 +1383,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1403,12 +1413,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1422,7 +1432,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1436,12 +1446,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1466,12 +1476,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1485,7 +1495,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1499,12 +1509,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1529,12 +1539,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1558,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1562,12 +1572,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1590,12 +1600,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>